<commit_message>
feat!: add feature to prepare import file for G2L nbr configuration
</commit_message>
<xml_diff>
--- a/neighbors/reports/templates/ToLTE.xlsx
+++ b/neighbors/reports/templates/ToLTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramalb/Desktop/nbr_temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramalb/Documents/kcell/python-projects/rantools-v2/neighbors/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDF7E45-6FF4-6047-A130-DF352B491284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29E832B-591F-124F-A02E-87398A2E273E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4315DCFD-10EB-D246-A07F-DE0188C7FE00}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>source cell</t>
   </si>
   <si>
-    <t>target cell</t>
+    <t>target earfcn</t>
   </si>
 </sst>
 </file>
@@ -122,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +162,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,7 +268,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,7 +410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,13 +421,13 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19">

</xml_diff>